<commit_message>
corrected spelling in excel
</commit_message>
<xml_diff>
--- a/input/reg_eq5d.xlsx
+++ b/input/reg_eq5d.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB4CCBC-A15C-4BF8-B125-94BF548C50A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5503AD4B-B91E-4AFD-9508-B4958390F37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A9A3AE8-34F1-4C3E-9682-3C69CFBA3626}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Che_pcs_cb</t>
+  </si>
+  <si>
+    <t>Dhe_pcs_cb</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +655,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>1.0699999999999999E-5</v>

</xml_diff>

<commit_message>
adding franks coefficients option
</commit_message>
<xml_diff>
--- a/input/reg_eq5d.xlsx
+++ b/input/reg_eq5d.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5503AD4B-B91E-4AFD-9508-B4958390F37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7731E325-0622-4050-B24A-A7B4DDB31076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A9A3AE8-34F1-4C3E-9682-3C69CFBA3626}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8A9A3AE8-34F1-4C3E-9682-3C69CFBA3626}"/>
   </bookViews>
   <sheets>
-    <sheet name="UK_EQ5D" sheetId="1" r:id="rId1"/>
+    <sheet name="UK_EQ5D_lawrence" sheetId="1" r:id="rId1"/>
+    <sheet name="UK_EQ5D_franks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -66,6 +67,21 @@
   </si>
   <si>
     <t>Dhe_pcs_cb</t>
+  </si>
+  <si>
+    <t>Dhe_pcs_c</t>
+  </si>
+  <si>
+    <t>Dhe_mcs_c</t>
+  </si>
+  <si>
+    <t>Dhe_pcs_c_sq</t>
+  </si>
+  <si>
+    <t>Dhe_mcs_c_sq</t>
+  </si>
+  <si>
+    <t>Dhe_mcs_c_times_pcs_c</t>
   </si>
 </sst>
 </file>
@@ -440,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCE0DF9-DC32-43B5-8DA4-440480E6714A}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +503,7 @@
         <v>-1.6983999999999999</v>
       </c>
       <c r="C2">
-        <v>2.0981522499999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -519,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>1.115136E-4</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -551,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>6.1008999999999902E-6</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -583,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>7.2899999999999998E-8</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -615,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <v>4.0000000000000001E-10</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -647,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>8.9999999999999999E-10</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -679,7 +695,258 @@
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>3.9999999999999999E-12</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8079D6CA-2355-449F-ADE5-FDF6FCFCC506}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0.84689999999999999</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1.261E-2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>7.5900000000000004E-3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>-9.0000000000000006E-5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>-1.4999999999999999E-4</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>-1.4999999999999999E-4</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>